<commit_message>
4.2 Cleaned Data in Earlier Files
</commit_message>
<xml_diff>
--- a/4.2 Cosmetics Inc - Data for Cleaning.xlsx
+++ b/4.2 Cosmetics Inc - Data for Cleaning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrsir\Downloads\Google-Data-Analytics-Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABBE2A7-5D35-433C-99A5-8207ED3E925B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B901FF1E-ED9B-4E06-A7AD-E9AB23957FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2490" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>Product Codes</t>
   </si>
@@ -243,6 +243,21 @@
   </si>
   <si>
     <t>CHEMD584</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>MID</t>
+  </si>
+  <si>
+    <t>CONCAT</t>
+  </si>
+  <si>
+    <t>TRIM</t>
   </si>
 </sst>
 </file>
@@ -264,18 +279,21 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -312,7 +330,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -327,23 +354,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -451,6 +462,40 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -465,15 +510,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A478D8EC-9B66-455E-9664-4D6D3D78ADA6}" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A478D8EC-9B66-455E-9664-4D6D3D78ADA6}" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:F31" xr:uid="{A478D8EC-9B66-455E-9664-4D6D3D78ADA6}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D9E54F16-7D01-4714-BEC2-3F7F0BC2DC3D}" name="Product Codes" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{BAFC1ACD-BB40-4F09-A4A9-95E88D5334FD}" name="Price" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E478553F-95B7-4CAC-A12C-69E4E0093BA3}" name="Client" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{5A8CDB80-CCE5-47E9-B26B-5E9159C4623D}" name="Client Code" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{C5B6C25A-0110-46FF-82FE-B2E3CD89B45D}" name="Orders" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{FB3C8FD7-A388-45CC-ABD3-9671E933F5FC}" name="Total" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{D9E54F16-7D01-4714-BEC2-3F7F0BC2DC3D}" name="Product Codes" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{BAFC1ACD-BB40-4F09-A4A9-95E88D5334FD}" name="Price" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{E478553F-95B7-4CAC-A12C-69E4E0093BA3}" name="Client" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{5A8CDB80-CCE5-47E9-B26B-5E9159C4623D}" name="Client Code" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{C5B6C25A-0110-46FF-82FE-B2E3CD89B45D}" name="Orders" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{FB3C8FD7-A388-45CC-ABD3-9671E933F5FC}" name="Total" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{304B8F02-D3D7-48B7-B145-49ACF25E2290}" name="Table2" displayName="Table2" ref="H1:L31" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="H1:L31" xr:uid="{304B8F02-D3D7-48B7-B145-49ACF25E2290}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B214695E-185D-4CC0-8E63-BD5031C8C95C}" name="LEFT">
+      <calculatedColumnFormula>LEFT(Table1[[#This Row],[Product Codes]],5)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{E508C0FE-AD8E-4C08-9DE1-F29F532C0D27}" name="RIGHT">
+      <calculatedColumnFormula>RIGHT(Table1[[#This Row],[Product Codes]],4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{1A13A10D-9320-4141-92B8-3AE3AD93B50A}" name="MID" dataDxfId="2">
+      <calculatedColumnFormula>MID(Table1[[#This Row],[Client Code]],4,2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{5C04396E-B744-433F-8BCC-55DEC69691A3}" name="CONCAT" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{AF222AD9-BD32-46B3-BE75-0B4A3A8400E4}" name="TRIM" dataDxfId="0">
+      <calculatedColumnFormula>TRIM(Table1[[#This Row],[Client]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -683,7 +752,7 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -695,6 +764,7 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
@@ -717,11 +787,21 @@
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -749,6 +829,26 @@
       <c r="F2" s="3">
         <v>1906.18</v>
       </c>
+      <c r="H2" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>51993</v>
+      </c>
+      <c r="I2" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Masc</v>
+      </c>
+      <c r="J2" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>NC</v>
+      </c>
+      <c r="K2" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>51993Masc</v>
+      </c>
+      <c r="L2" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Candy's Beauty Supply</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -769,6 +869,26 @@
       <c r="F3" s="3">
         <v>2202.48</v>
       </c>
+      <c r="H3" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>49631</v>
+      </c>
+      <c r="I3" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J3" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>VA</v>
+      </c>
+      <c r="K3" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>49631Foun</v>
+      </c>
+      <c r="L3" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rockland's</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -789,6 +909,26 @@
       <c r="F4" s="3">
         <v>5108.92</v>
       </c>
+      <c r="H4" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>42292</v>
+      </c>
+      <c r="I4" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Glos</v>
+      </c>
+      <c r="J4" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>MD</v>
+      </c>
+      <c r="K4" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>42292Glos</v>
+      </c>
+      <c r="L4" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rudiger Pharmacy</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -809,6 +949,26 @@
       <c r="F5" s="3">
         <v>1758.68</v>
       </c>
+      <c r="H5" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>86661</v>
+      </c>
+      <c r="I5" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Shad</v>
+      </c>
+      <c r="J5" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K5" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>86661Shad</v>
+      </c>
+      <c r="L5" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -829,6 +989,26 @@
       <c r="F6" s="3">
         <v>397</v>
       </c>
+      <c r="H6" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>49541</v>
+      </c>
+      <c r="I6" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Eyel</v>
+      </c>
+      <c r="J6" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>VA</v>
+      </c>
+      <c r="K6" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>49541Eyel</v>
+      </c>
+      <c r="L6" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rockland's</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -849,6 +1029,26 @@
       <c r="F7" s="3">
         <v>9132.61</v>
       </c>
+      <c r="H7" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>58337</v>
+      </c>
+      <c r="I7" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J7" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>NC</v>
+      </c>
+      <c r="K7" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>58337Foun</v>
+      </c>
+      <c r="L7" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Candy's Beauty Supply</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -869,6 +1069,26 @@
       <c r="F8" s="3">
         <v>795.24000000000012</v>
       </c>
+      <c r="H8" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>40014</v>
+      </c>
+      <c r="I8" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Masc</v>
+      </c>
+      <c r="J8" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K8" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>40014Masc</v>
+      </c>
+      <c r="L8" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -889,6 +1109,26 @@
       <c r="F9" s="3">
         <v>1659.45</v>
       </c>
+      <c r="H9" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>86139</v>
+      </c>
+      <c r="I9" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Lips</v>
+      </c>
+      <c r="J9" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>NC</v>
+      </c>
+      <c r="K9" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>86139Lips</v>
+      </c>
+      <c r="L9" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Candy's Beauty Supply</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -909,6 +1149,26 @@
       <c r="F10" s="3">
         <v>9392.5</v>
       </c>
+      <c r="H10" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>69601</v>
+      </c>
+      <c r="I10" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Exfo</v>
+      </c>
+      <c r="J10" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>VA</v>
+      </c>
+      <c r="K10" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>69601Exfo</v>
+      </c>
+      <c r="L10" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rockland's</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -929,6 +1189,26 @@
       <c r="F11" s="3">
         <v>1281.02</v>
       </c>
+      <c r="H11" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>25331</v>
+      </c>
+      <c r="I11" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Glos</v>
+      </c>
+      <c r="J11" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>VA</v>
+      </c>
+      <c r="K11" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>25331Glos</v>
+      </c>
+      <c r="L11" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rockland's</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -950,6 +1230,26 @@
         <f>(B12*E12)</f>
         <v>8307.25</v>
       </c>
+      <c r="H12" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>85021</v>
+      </c>
+      <c r="I12" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J12" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>MD</v>
+      </c>
+      <c r="K12" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>85021Foun</v>
+      </c>
+      <c r="L12" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rudiger Pharmacy</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -970,6 +1270,26 @@
       <c r="F13" s="3">
         <v>5047.95</v>
       </c>
+      <c r="H13" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>69030</v>
+      </c>
+      <c r="I13" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Masc</v>
+      </c>
+      <c r="J13" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K13" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>69030Masc</v>
+      </c>
+      <c r="L13" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -990,6 +1310,26 @@
       <c r="F14" s="3">
         <v>914.94</v>
       </c>
+      <c r="H14" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>13230</v>
+      </c>
+      <c r="I14" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Masc</v>
+      </c>
+      <c r="J14" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>VA</v>
+      </c>
+      <c r="K14" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>13230Masc</v>
+      </c>
+      <c r="L14" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rockland's</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -1010,6 +1350,26 @@
       <c r="F15" s="3">
         <v>2957.04</v>
       </c>
+      <c r="H15" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>91559</v>
+      </c>
+      <c r="I15" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Eyel</v>
+      </c>
+      <c r="J15" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>NC</v>
+      </c>
+      <c r="K15" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>91559Eyel</v>
+      </c>
+      <c r="L15" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Candy's Beauty Supply</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1030,8 +1390,28 @@
       <c r="F16" s="3">
         <v>9611.82</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H16" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>62289</v>
+      </c>
+      <c r="I16" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Masc</v>
+      </c>
+      <c r="J16" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K16" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>62289Masc</v>
+      </c>
+      <c r="L16" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -1050,8 +1430,28 @@
       <c r="F17" s="3">
         <v>4597.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>64762</v>
+      </c>
+      <c r="I17" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J17" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>MD</v>
+      </c>
+      <c r="K17" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>64762Foun</v>
+      </c>
+      <c r="L17" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rudiger Pharmacy</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>42</v>
       </c>
@@ -1070,8 +1470,28 @@
       <c r="F18" s="3">
         <v>3036.88</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>52341</v>
+      </c>
+      <c r="I18" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J18" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K18" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>52341Foun</v>
+      </c>
+      <c r="L18" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -1090,8 +1510,28 @@
       <c r="F19" s="3">
         <v>8105.78</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>68713</v>
+      </c>
+      <c r="I19" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Exfo</v>
+      </c>
+      <c r="J19" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>VA</v>
+      </c>
+      <c r="K19" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>68713Exfo</v>
+      </c>
+      <c r="L19" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rockland's</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -1110,8 +1550,28 @@
       <c r="F20" s="3">
         <v>2233.98</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>35073</v>
+      </c>
+      <c r="I20" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J20" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K20" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>35073Foun</v>
+      </c>
+      <c r="L20" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
@@ -1130,8 +1590,28 @@
       <c r="F21" s="3">
         <v>6967.6200000000008</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>17691</v>
+      </c>
+      <c r="I21" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Masc</v>
+      </c>
+      <c r="J21" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K21" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>17691Masc</v>
+      </c>
+      <c r="L21" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
@@ -1150,8 +1630,28 @@
       <c r="F22" s="3">
         <v>3227</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>03485</v>
+      </c>
+      <c r="I22" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Eyel</v>
+      </c>
+      <c r="J22" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>MD</v>
+      </c>
+      <c r="K22" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>03485Eyel</v>
+      </c>
+      <c r="L22" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rudiger Pharmacy</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -1170,8 +1670,28 @@
       <c r="F23" s="3">
         <v>1753.46</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H23" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>26156</v>
+      </c>
+      <c r="I23" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J23" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>NC</v>
+      </c>
+      <c r="K23" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>26156Foun</v>
+      </c>
+      <c r="L23" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Candy's Beauty Supply</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -1190,8 +1710,28 @@
       <c r="F24" s="3">
         <v>3455.64</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>75112</v>
+      </c>
+      <c r="I24" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J24" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K24" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>75112Foun</v>
+      </c>
+      <c r="L24" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
@@ -1210,8 +1750,28 @@
       <c r="F25" s="3">
         <v>6062.14</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H25" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>96799</v>
+      </c>
+      <c r="I25" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J25" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>MD</v>
+      </c>
+      <c r="K25" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>96799Foun</v>
+      </c>
+      <c r="L25" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rudiger Pharmacy</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>58</v>
       </c>
@@ -1230,8 +1790,28 @@
       <c r="F26" s="3">
         <v>974.25</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>20559</v>
+      </c>
+      <c r="I26" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Shad</v>
+      </c>
+      <c r="J26" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K26" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>20559Shad</v>
+      </c>
+      <c r="L26" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>60</v>
       </c>
@@ -1250,8 +1830,28 @@
       <c r="F27" s="3">
         <v>12762.36</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>32729</v>
+      </c>
+      <c r="I27" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Masc</v>
+      </c>
+      <c r="J27" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>SC</v>
+      </c>
+      <c r="K27" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>32729Masc</v>
+      </c>
+      <c r="L27" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Elizabethtown Supply</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>62</v>
       </c>
@@ -1270,8 +1870,28 @@
       <c r="F28" s="3">
         <v>6132.2800000000007</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H28" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>63094</v>
+      </c>
+      <c r="I28" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Exfo</v>
+      </c>
+      <c r="J28" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>NC</v>
+      </c>
+      <c r="K28" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>63094Exfo</v>
+      </c>
+      <c r="L28" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Candy's Beauty Supply</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
@@ -1290,8 +1910,28 @@
       <c r="F29" s="3">
         <v>5780.04</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H29" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>61207</v>
+      </c>
+      <c r="I29" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Foun</v>
+      </c>
+      <c r="J29" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>MD</v>
+      </c>
+      <c r="K29" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>61207Foun</v>
+      </c>
+      <c r="L29" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rudiger Pharmacy</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
@@ -1310,8 +1950,28 @@
       <c r="F30" s="3">
         <v>5695.95</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H30" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>17269</v>
+      </c>
+      <c r="I30" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Masc</v>
+      </c>
+      <c r="J30" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>VA</v>
+      </c>
+      <c r="K30" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>17269Masc</v>
+      </c>
+      <c r="L30" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rockland's</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
@@ -1330,11 +1990,32 @@
       <c r="F31" s="3">
         <v>15671.28</v>
       </c>
+      <c r="H31" t="str">
+        <f>LEFT(Table1[[#This Row],[Product Codes]],5)</f>
+        <v>15143</v>
+      </c>
+      <c r="I31" t="str">
+        <f>RIGHT(Table1[[#This Row],[Product Codes]],4)</f>
+        <v>Exfo</v>
+      </c>
+      <c r="J31" t="str">
+        <f>MID(Table1[[#This Row],[Client Code]],4,2)</f>
+        <v>MD</v>
+      </c>
+      <c r="K31" t="str">
+        <f>_xlfn.CONCAT(Table2[[#This Row],[LEFT]],Table2[[#This Row],[RIGHT]])</f>
+        <v>15143Exfo</v>
+      </c>
+      <c r="L31" t="str">
+        <f>TRIM(Table1[[#This Row],[Client]])</f>
+        <v>Rudiger Pharmacy</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>